<commit_message>
functional MLSs allround, functional whitenoise, sweep, pure sine etc.
</commit_message>
<xml_diff>
--- a/Project/Kode/MLSGeneratorAverageTimes.xlsx
+++ b/Project/Kode/MLSGeneratorAverageTimes.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Christian Lykke\Documents\Skole\Aalborg Universitet\ESD6\Project\Kode\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{850AB31B-AB6F-43D2-9927-D84BDE0512C2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2049A843-0F06-447A-ACD8-B95C08D5D270}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{77718FEC-CCAD-4B45-B589-CCDFD0FA239E}"/>
+    <workbookView xWindow="19200" yWindow="-21600" windowWidth="19200" windowHeight="21000" xr2:uid="{77718FEC-CCAD-4B45-B589-CCDFD0FA239E}"/>
   </bookViews>
   <sheets>
     <sheet name="Ark1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
   <si>
     <t>Bitnumber</t>
   </si>
@@ -70,21 +70,12 @@
   <si>
     <t>Converter to hours</t>
   </si>
-  <si>
-    <t>Audible?</t>
-  </si>
-  <si>
-    <t>N</t>
-  </si>
-  <si>
-    <t>Y</t>
-  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -94,6 +85,12 @@
     </font>
     <font>
       <sz val="8"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -302,7 +299,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -316,7 +313,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -654,15 +657,15 @@
   <dimension ref="A1:L32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L6" sqref="L6"/>
+      <selection activeCell="L1" sqref="L1:L22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="9.33203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="10" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11" bestFit="1" customWidth="1"/>
-    <col min="5" max="6" width="5.44140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12" bestFit="1" customWidth="1"/>
+    <col min="4" max="6" width="10" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="11" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="14" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="12.33203125" bestFit="1" customWidth="1"/>
@@ -704,9 +707,7 @@
       <c r="K1" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="13" t="s">
-        <v>11</v>
-      </c>
+      <c r="L1" s="13"/>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A2" s="7">
@@ -721,30 +722,31 @@
       <c r="D2" s="8">
         <v>1</v>
       </c>
-      <c r="E2" s="8"/>
-      <c r="F2" s="8"/>
+      <c r="E2" s="8">
+        <v>1</v>
+      </c>
+      <c r="F2" s="8">
+        <v>1</v>
+      </c>
       <c r="G2" s="8">
         <f>SUM(B2:F2)/5</f>
-        <v>0.6</v>
+        <v>1</v>
       </c>
       <c r="H2" s="8">
         <f>G2/1000</f>
-        <v>5.9999999999999995E-4</v>
-      </c>
-      <c r="I2" s="8">
+        <v>1E-3</v>
+      </c>
+      <c r="I2" s="15">
         <f>H2/1000</f>
-        <v>5.9999999999999997E-7</v>
+        <v>9.9999999999999995E-7</v>
       </c>
       <c r="J2" s="8">
         <f>I2/60</f>
-        <v>1E-8</v>
+        <v>1.6666666666666667E-8</v>
       </c>
       <c r="K2" s="9">
         <f>J2/60</f>
-        <v>1.6666666666666666E-10</v>
-      </c>
-      <c r="L2" t="s">
-        <v>12</v>
+        <v>2.7777777777777777E-10</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.3">
@@ -760,30 +762,31 @@
       <c r="D3" s="1">
         <v>2</v>
       </c>
-      <c r="E3" s="1"/>
-      <c r="F3" s="1"/>
+      <c r="E3" s="1">
+        <v>1</v>
+      </c>
+      <c r="F3" s="1">
+        <v>1</v>
+      </c>
       <c r="G3" s="1">
-        <f t="shared" ref="G3:G32" si="0">SUM(B3:F3)/5</f>
-        <v>1.2</v>
+        <f t="shared" ref="G3:G24" si="0">SUM(B3:F3)/5</f>
+        <v>1.6</v>
       </c>
       <c r="H3" s="1">
         <f t="shared" ref="H3:I3" si="1">G3/1000</f>
-        <v>1.1999999999999999E-3</v>
-      </c>
-      <c r="I3" s="1">
+        <v>1.6000000000000001E-3</v>
+      </c>
+      <c r="I3" s="16">
         <f t="shared" si="1"/>
-        <v>1.1999999999999999E-6</v>
+        <v>1.6000000000000001E-6</v>
       </c>
       <c r="J3" s="1">
         <f t="shared" ref="J3:K3" si="2">I3/60</f>
-        <v>2E-8</v>
+        <v>2.6666666666666671E-8</v>
       </c>
       <c r="K3" s="3">
         <f t="shared" si="2"/>
-        <v>3.3333333333333332E-10</v>
-      </c>
-      <c r="L3" t="s">
-        <v>12</v>
+        <v>4.4444444444444453E-10</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.3">
@@ -799,30 +802,31 @@
       <c r="D4" s="1">
         <v>2</v>
       </c>
-      <c r="E4" s="1"/>
-      <c r="F4" s="1"/>
+      <c r="E4" s="1">
+        <v>1</v>
+      </c>
+      <c r="F4" s="1">
+        <v>1</v>
+      </c>
       <c r="G4" s="1">
         <f t="shared" si="0"/>
-        <v>1.2</v>
+        <v>1.6</v>
       </c>
       <c r="H4" s="1">
         <f t="shared" ref="H4:I4" si="3">G4/1000</f>
-        <v>1.1999999999999999E-3</v>
-      </c>
-      <c r="I4" s="1">
+        <v>1.6000000000000001E-3</v>
+      </c>
+      <c r="I4" s="16">
         <f t="shared" si="3"/>
-        <v>1.1999999999999999E-6</v>
+        <v>1.6000000000000001E-6</v>
       </c>
       <c r="J4" s="1">
         <f t="shared" ref="J4:K4" si="4">I4/60</f>
-        <v>2E-8</v>
+        <v>2.6666666666666671E-8</v>
       </c>
       <c r="K4" s="3">
         <f t="shared" si="4"/>
-        <v>3.3333333333333332E-10</v>
-      </c>
-      <c r="L4" t="s">
-        <v>12</v>
+        <v>4.4444444444444453E-10</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.3">
@@ -838,30 +842,31 @@
       <c r="D5" s="1">
         <v>3</v>
       </c>
-      <c r="E5" s="1"/>
-      <c r="F5" s="1"/>
+      <c r="E5" s="1">
+        <v>2</v>
+      </c>
+      <c r="F5" s="1">
+        <v>2</v>
+      </c>
       <c r="G5" s="1">
         <f t="shared" si="0"/>
-        <v>1.8</v>
+        <v>2.6</v>
       </c>
       <c r="H5" s="1">
         <f t="shared" ref="H5:I5" si="5">G5/1000</f>
-        <v>1.8E-3</v>
-      </c>
-      <c r="I5" s="1">
+        <v>2.5999999999999999E-3</v>
+      </c>
+      <c r="I5" s="16">
         <f t="shared" si="5"/>
-        <v>1.7999999999999999E-6</v>
+        <v>2.5999999999999997E-6</v>
       </c>
       <c r="J5" s="1">
         <f t="shared" ref="J5:K5" si="6">I5/60</f>
-        <v>2.9999999999999997E-8</v>
+        <v>4.3333333333333331E-8</v>
       </c>
       <c r="K5" s="3">
         <f t="shared" si="6"/>
-        <v>4.9999999999999993E-10</v>
-      </c>
-      <c r="L5" t="s">
-        <v>12</v>
+        <v>7.2222222222222214E-10</v>
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.3">
@@ -877,30 +882,31 @@
       <c r="D6" s="1">
         <v>5</v>
       </c>
-      <c r="E6" s="1"/>
-      <c r="F6" s="1"/>
+      <c r="E6" s="1">
+        <v>4</v>
+      </c>
+      <c r="F6" s="1">
+        <v>4</v>
+      </c>
       <c r="G6" s="1">
         <f t="shared" si="0"/>
-        <v>3</v>
+        <v>4.5999999999999996</v>
       </c>
       <c r="H6" s="1">
         <f t="shared" ref="H6:I6" si="7">G6/1000</f>
-        <v>3.0000000000000001E-3</v>
-      </c>
-      <c r="I6" s="1">
+        <v>4.5999999999999999E-3</v>
+      </c>
+      <c r="I6" s="16">
         <f t="shared" si="7"/>
-        <v>3.0000000000000001E-6</v>
+        <v>4.6E-6</v>
       </c>
       <c r="J6" s="1">
         <f t="shared" ref="J6:K6" si="8">I6/60</f>
-        <v>5.0000000000000004E-8</v>
+        <v>7.6666666666666665E-8</v>
       </c>
       <c r="K6" s="3">
         <f t="shared" si="8"/>
-        <v>8.3333333333333345E-10</v>
-      </c>
-      <c r="L6" t="s">
-        <v>12</v>
+        <v>1.2777777777777778E-9</v>
       </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.3">
@@ -916,30 +922,31 @@
       <c r="D7" s="1">
         <v>10</v>
       </c>
-      <c r="E7" s="1"/>
-      <c r="F7" s="1"/>
+      <c r="E7" s="1">
+        <v>8</v>
+      </c>
+      <c r="F7" s="1">
+        <v>8</v>
+      </c>
       <c r="G7" s="1">
         <f t="shared" si="0"/>
-        <v>5.2</v>
+        <v>8.4</v>
       </c>
       <c r="H7" s="1">
         <f t="shared" ref="H7:I7" si="9">G7/1000</f>
-        <v>5.1999999999999998E-3</v>
-      </c>
-      <c r="I7" s="1">
+        <v>8.4000000000000012E-3</v>
+      </c>
+      <c r="I7" s="16">
         <f t="shared" si="9"/>
-        <v>5.1999999999999993E-6</v>
+        <v>8.4000000000000009E-6</v>
       </c>
       <c r="J7" s="1">
         <f t="shared" ref="J7:K7" si="10">I7/60</f>
-        <v>8.6666666666666662E-8</v>
+        <v>1.4000000000000001E-7</v>
       </c>
       <c r="K7" s="3">
         <f t="shared" si="10"/>
-        <v>1.4444444444444443E-9</v>
-      </c>
-      <c r="L7" t="s">
-        <v>13</v>
+        <v>2.3333333333333335E-9</v>
       </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.3">
@@ -955,30 +962,31 @@
       <c r="D8" s="1">
         <v>15</v>
       </c>
-      <c r="E8" s="1"/>
-      <c r="F8" s="1"/>
+      <c r="E8" s="1">
+        <v>14</v>
+      </c>
+      <c r="F8" s="1">
+        <v>14</v>
+      </c>
       <c r="G8" s="1">
         <f t="shared" si="0"/>
-        <v>9</v>
+        <v>14.6</v>
       </c>
       <c r="H8" s="1">
         <f t="shared" ref="H8:I8" si="11">G8/1000</f>
-        <v>8.9999999999999993E-3</v>
-      </c>
-      <c r="I8" s="1">
+        <v>1.46E-2</v>
+      </c>
+      <c r="I8" s="16">
         <f t="shared" si="11"/>
-        <v>8.9999999999999985E-6</v>
+        <v>1.4600000000000001E-5</v>
       </c>
       <c r="J8" s="1">
         <f t="shared" ref="J8:K8" si="12">I8/60</f>
-        <v>1.4999999999999997E-7</v>
+        <v>2.4333333333333337E-7</v>
       </c>
       <c r="K8" s="3">
         <f t="shared" si="12"/>
-        <v>2.4999999999999996E-9</v>
-      </c>
-      <c r="L8" t="s">
-        <v>13</v>
+        <v>4.0555555555555558E-9</v>
       </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.3">
@@ -994,30 +1002,31 @@
       <c r="D9" s="1">
         <v>28</v>
       </c>
-      <c r="E9" s="1"/>
-      <c r="F9" s="1"/>
+      <c r="E9" s="1">
+        <v>27</v>
+      </c>
+      <c r="F9" s="1">
+        <v>27</v>
+      </c>
       <c r="G9" s="1">
         <f t="shared" si="0"/>
-        <v>16.8</v>
+        <v>27.6</v>
       </c>
       <c r="H9" s="1">
         <f t="shared" ref="H9:I9" si="13">G9/1000</f>
-        <v>1.6800000000000002E-2</v>
-      </c>
-      <c r="I9" s="1">
+        <v>2.7600000000000003E-2</v>
+      </c>
+      <c r="I9" s="16">
         <f t="shared" si="13"/>
-        <v>1.6800000000000002E-5</v>
+        <v>2.7600000000000003E-5</v>
       </c>
       <c r="J9" s="1">
         <f t="shared" ref="J9:K9" si="14">I9/60</f>
-        <v>2.8000000000000002E-7</v>
+        <v>4.6000000000000004E-7</v>
       </c>
       <c r="K9" s="3">
         <f t="shared" si="14"/>
-        <v>4.6666666666666671E-9</v>
-      </c>
-      <c r="L9" t="s">
-        <v>13</v>
+        <v>7.6666666666666675E-9</v>
       </c>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.3">
@@ -1033,30 +1042,31 @@
       <c r="D10" s="1">
         <v>53</v>
       </c>
-      <c r="E10" s="1"/>
-      <c r="F10" s="1"/>
+      <c r="E10" s="1">
+        <v>53</v>
+      </c>
+      <c r="F10" s="1">
+        <v>53</v>
+      </c>
       <c r="G10" s="1">
         <f t="shared" si="0"/>
-        <v>31.8</v>
+        <v>53</v>
       </c>
       <c r="H10" s="1">
         <f t="shared" ref="H10:I10" si="15">G10/1000</f>
-        <v>3.1800000000000002E-2</v>
-      </c>
-      <c r="I10" s="1">
+        <v>5.2999999999999999E-2</v>
+      </c>
+      <c r="I10" s="16">
         <f t="shared" si="15"/>
-        <v>3.18E-5</v>
+        <v>5.3000000000000001E-5</v>
       </c>
       <c r="J10" s="1">
         <f t="shared" ref="J10:K10" si="16">I10/60</f>
-        <v>5.3000000000000001E-7</v>
+        <v>8.8333333333333338E-7</v>
       </c>
       <c r="K10" s="3">
         <f t="shared" si="16"/>
-        <v>8.833333333333333E-9</v>
-      </c>
-      <c r="L10" t="s">
-        <v>13</v>
+        <v>1.4722222222222223E-8</v>
       </c>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.3">
@@ -1072,30 +1082,31 @@
       <c r="D11" s="1">
         <v>106</v>
       </c>
-      <c r="E11" s="1"/>
-      <c r="F11" s="1"/>
+      <c r="E11" s="1">
+        <v>106</v>
+      </c>
+      <c r="F11" s="1">
+        <v>106</v>
+      </c>
       <c r="G11" s="1">
         <f t="shared" si="0"/>
-        <v>64</v>
+        <v>106.4</v>
       </c>
       <c r="H11" s="1">
         <f t="shared" ref="H11:I11" si="17">G11/1000</f>
-        <v>6.4000000000000001E-2</v>
-      </c>
-      <c r="I11" s="1">
+        <v>0.10640000000000001</v>
+      </c>
+      <c r="I11" s="16">
         <f t="shared" si="17"/>
-        <v>6.3999999999999997E-5</v>
+        <v>1.0640000000000001E-4</v>
       </c>
       <c r="J11" s="1">
         <f t="shared" ref="J11:K11" si="18">I11/60</f>
-        <v>1.0666666666666667E-6</v>
+        <v>1.7733333333333334E-6</v>
       </c>
       <c r="K11" s="3">
         <f t="shared" si="18"/>
-        <v>1.7777777777777777E-8</v>
-      </c>
-      <c r="L11" t="s">
-        <v>13</v>
+        <v>2.9555555555555557E-8</v>
       </c>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.3">
@@ -1111,30 +1122,31 @@
       <c r="D12" s="1">
         <v>208</v>
       </c>
-      <c r="E12" s="1"/>
-      <c r="F12" s="1"/>
+      <c r="E12" s="1">
+        <v>208</v>
+      </c>
+      <c r="F12" s="1">
+        <v>208</v>
+      </c>
       <c r="G12" s="1">
         <f t="shared" si="0"/>
-        <v>125</v>
+        <v>208.2</v>
       </c>
       <c r="H12" s="1">
         <f t="shared" ref="H12:I12" si="19">G12/1000</f>
-        <v>0.125</v>
-      </c>
-      <c r="I12" s="1">
+        <v>0.2082</v>
+      </c>
+      <c r="I12" s="16">
         <f t="shared" si="19"/>
-        <v>1.25E-4</v>
+        <v>2.0819999999999999E-4</v>
       </c>
       <c r="J12" s="1">
         <f t="shared" ref="J12:K12" si="20">I12/60</f>
-        <v>2.0833333333333334E-6</v>
+        <v>3.4699999999999998E-6</v>
       </c>
       <c r="K12" s="3">
         <f t="shared" si="20"/>
-        <v>3.4722222222222227E-8</v>
-      </c>
-      <c r="L12" t="s">
-        <v>13</v>
+        <v>5.7833333333333328E-8</v>
       </c>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.3">
@@ -1150,30 +1162,31 @@
       <c r="D13" s="1">
         <v>418</v>
       </c>
-      <c r="E13" s="1"/>
-      <c r="F13" s="1"/>
+      <c r="E13" s="1">
+        <v>419</v>
+      </c>
+      <c r="F13" s="1">
+        <v>418</v>
+      </c>
       <c r="G13" s="1">
         <f t="shared" si="0"/>
-        <v>251</v>
+        <v>418.4</v>
       </c>
       <c r="H13" s="1">
         <f t="shared" ref="H13:I13" si="21">G13/1000</f>
-        <v>0.251</v>
-      </c>
-      <c r="I13" s="1">
+        <v>0.41839999999999999</v>
+      </c>
+      <c r="I13" s="16">
         <f t="shared" si="21"/>
-        <v>2.5099999999999998E-4</v>
+        <v>4.1839999999999998E-4</v>
       </c>
       <c r="J13" s="1">
         <f t="shared" ref="J13:K13" si="22">I13/60</f>
-        <v>4.1833333333333328E-6</v>
+        <v>6.9733333333333332E-6</v>
       </c>
       <c r="K13" s="3">
         <f t="shared" si="22"/>
-        <v>6.9722222222222209E-8</v>
-      </c>
-      <c r="L13" t="s">
-        <v>13</v>
+        <v>1.1622222222222222E-7</v>
       </c>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.3">
@@ -1189,30 +1202,31 @@
       <c r="D14" s="1">
         <v>142186</v>
       </c>
-      <c r="E14" s="1"/>
-      <c r="F14" s="1"/>
+      <c r="E14" s="1">
+        <v>141986</v>
+      </c>
+      <c r="F14" s="1">
+        <v>141048</v>
+      </c>
       <c r="G14" s="1">
         <f t="shared" si="0"/>
-        <v>84543.6</v>
+        <v>141150.39999999999</v>
       </c>
       <c r="H14" s="1">
         <f t="shared" ref="H14:I14" si="23">G14/1000</f>
-        <v>84.543600000000012</v>
-      </c>
-      <c r="I14" s="1">
+        <v>141.15039999999999</v>
+      </c>
+      <c r="I14" s="16">
         <f t="shared" si="23"/>
-        <v>8.454360000000001E-2</v>
+        <v>0.14115039999999998</v>
       </c>
       <c r="J14" s="1">
         <f t="shared" ref="J14:K14" si="24">I14/60</f>
-        <v>1.4090600000000002E-3</v>
+        <v>2.3525066666666662E-3</v>
       </c>
       <c r="K14" s="3">
         <f t="shared" si="24"/>
-        <v>2.3484333333333335E-5</v>
-      </c>
-      <c r="L14" t="s">
-        <v>13</v>
+        <v>3.9208444444444438E-5</v>
       </c>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.3">
@@ -1228,30 +1242,31 @@
       <c r="D15" s="1">
         <v>512195</v>
       </c>
-      <c r="E15" s="1"/>
-      <c r="F15" s="1"/>
+      <c r="E15" s="1">
+        <v>512196</v>
+      </c>
+      <c r="F15" s="1">
+        <v>512195</v>
+      </c>
       <c r="G15" s="1">
         <f t="shared" si="0"/>
-        <v>307461</v>
+        <v>512339.20000000001</v>
       </c>
       <c r="H15" s="1">
         <f t="shared" ref="H15:I15" si="25">G15/1000</f>
-        <v>307.46100000000001</v>
-      </c>
-      <c r="I15" s="1">
+        <v>512.33920000000001</v>
+      </c>
+      <c r="I15" s="16">
         <f t="shared" si="25"/>
-        <v>0.30746100000000004</v>
+        <v>0.51233919999999999</v>
       </c>
       <c r="J15" s="1">
         <f t="shared" ref="J15:K15" si="26">I15/60</f>
-        <v>5.1243500000000006E-3</v>
+        <v>8.5389866666666665E-3</v>
       </c>
       <c r="K15" s="3">
         <f t="shared" si="26"/>
-        <v>8.5405833333333342E-5</v>
-      </c>
-      <c r="L15" t="s">
-        <v>13</v>
+        <v>1.4231644444444443E-4</v>
       </c>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.3">
@@ -1267,33 +1282,34 @@
       <c r="D16" s="1">
         <v>1255234</v>
       </c>
-      <c r="E16" s="1"/>
-      <c r="F16" s="1"/>
+      <c r="E16" s="1">
+        <v>1255234</v>
+      </c>
+      <c r="F16" s="1">
+        <v>1255234</v>
+      </c>
       <c r="G16" s="1">
         <f t="shared" si="0"/>
-        <v>753140.2</v>
+        <v>1255233.8</v>
       </c>
       <c r="H16" s="1">
         <f t="shared" ref="H16:I16" si="27">G16/1000</f>
-        <v>753.14019999999994</v>
-      </c>
-      <c r="I16" s="1">
+        <v>1255.2338</v>
+      </c>
+      <c r="I16" s="16">
         <f t="shared" si="27"/>
-        <v>0.75314019999999993</v>
+        <v>1.2552338000000001</v>
       </c>
       <c r="J16" s="1">
         <f t="shared" ref="J16:K16" si="28">I16/60</f>
-        <v>1.2552336666666665E-2</v>
+        <v>2.0920563333333333E-2</v>
       </c>
       <c r="K16" s="3">
         <f t="shared" si="28"/>
-        <v>2.0920561111111108E-4</v>
-      </c>
-      <c r="L16" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.3">
+        <v>3.4867605555555557E-4</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A17" s="2">
         <v>17</v>
       </c>
@@ -1306,33 +1322,34 @@
       <c r="D17" s="1">
         <v>2741311</v>
       </c>
-      <c r="E17" s="1"/>
-      <c r="F17" s="1"/>
+      <c r="E17" s="1">
+        <v>2741311</v>
+      </c>
+      <c r="F17" s="1">
+        <v>2741311</v>
+      </c>
       <c r="G17" s="1">
         <f t="shared" si="0"/>
-        <v>1644786.4</v>
+        <v>2741310.8</v>
       </c>
       <c r="H17" s="1">
         <f t="shared" ref="H17:I17" si="29">G17/1000</f>
-        <v>1644.7864</v>
-      </c>
-      <c r="I17" s="1">
+        <v>2741.3107999999997</v>
+      </c>
+      <c r="I17" s="16">
         <f t="shared" si="29"/>
-        <v>1.6447863999999999</v>
+        <v>2.7413107999999999</v>
       </c>
       <c r="J17" s="1">
         <f t="shared" ref="J17:K17" si="30">I17/60</f>
-        <v>2.7413106666666666E-2</v>
+        <v>4.5688513333333333E-2</v>
       </c>
       <c r="K17" s="3">
         <f t="shared" si="30"/>
-        <v>4.5688511111111112E-4</v>
-      </c>
-      <c r="L17" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.3">
+        <v>7.6147522222222224E-4</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A18" s="2">
         <v>18</v>
       </c>
@@ -1345,33 +1362,34 @@
       <c r="D18" s="1">
         <v>5713465</v>
       </c>
-      <c r="E18" s="1"/>
-      <c r="F18" s="1"/>
+      <c r="E18" s="1">
+        <v>5713466</v>
+      </c>
+      <c r="F18" s="1">
+        <v>5713465</v>
+      </c>
       <c r="G18" s="1">
         <f t="shared" si="0"/>
-        <v>3428078.8</v>
+        <v>5713465</v>
       </c>
       <c r="H18" s="1">
         <f t="shared" ref="H18:I18" si="31">G18/1000</f>
-        <v>3428.0787999999998</v>
-      </c>
-      <c r="I18" s="1">
+        <v>5713.4650000000001</v>
+      </c>
+      <c r="I18" s="16">
         <f t="shared" si="31"/>
-        <v>3.4280787999999998</v>
+        <v>5.7134650000000002</v>
       </c>
       <c r="J18" s="1">
         <f t="shared" ref="J18:K18" si="32">I18/60</f>
-        <v>5.7134646666666664E-2</v>
+        <v>9.5224416666666672E-2</v>
       </c>
       <c r="K18" s="3">
         <f t="shared" si="32"/>
-        <v>9.5224411111111107E-4</v>
-      </c>
-      <c r="L18" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.3">
+        <v>1.5870736111111112E-3</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A19" s="2">
         <v>19</v>
       </c>
@@ -1384,30 +1402,34 @@
       <c r="D19" s="1">
         <v>11657773</v>
       </c>
-      <c r="E19" s="1"/>
-      <c r="F19" s="1"/>
+      <c r="E19" s="1">
+        <v>11657773</v>
+      </c>
+      <c r="F19" s="1">
+        <v>11657773</v>
+      </c>
       <c r="G19" s="1">
         <f t="shared" si="0"/>
-        <v>6994663.7999999998</v>
+        <v>11657773</v>
       </c>
       <c r="H19" s="1">
         <f t="shared" ref="H19:I19" si="33">G19/1000</f>
-        <v>6994.6638000000003</v>
-      </c>
-      <c r="I19" s="1">
+        <v>11657.772999999999</v>
+      </c>
+      <c r="I19" s="16">
         <f t="shared" si="33"/>
-        <v>6.9946638000000005</v>
+        <v>11.657772999999999</v>
       </c>
       <c r="J19" s="1">
         <f t="shared" ref="J19:K19" si="34">I19/60</f>
-        <v>0.11657773</v>
+        <v>0.19429621666666666</v>
       </c>
       <c r="K19" s="3">
         <f t="shared" si="34"/>
-        <v>1.9429621666666667E-3</v>
-      </c>
-    </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.3">
+        <v>3.2382702777777775E-3</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A20" s="2">
         <v>20</v>
       </c>
@@ -1420,30 +1442,34 @@
       <c r="D20" s="1">
         <v>23546389</v>
       </c>
-      <c r="E20" s="1"/>
-      <c r="F20" s="1"/>
+      <c r="E20" s="1">
+        <v>23546390</v>
+      </c>
+      <c r="F20" s="1">
+        <v>23546390</v>
+      </c>
       <c r="G20" s="1">
         <f t="shared" si="0"/>
-        <v>14127833.6</v>
+        <v>23546389.600000001</v>
       </c>
       <c r="H20" s="1">
         <f t="shared" ref="H20:I20" si="35">G20/1000</f>
-        <v>14127.8336</v>
-      </c>
-      <c r="I20" s="1">
+        <v>23546.389600000002</v>
+      </c>
+      <c r="I20" s="16">
         <f t="shared" si="35"/>
-        <v>14.127833600000001</v>
+        <v>23.546389600000001</v>
       </c>
       <c r="J20" s="1">
         <f t="shared" ref="J20:K20" si="36">I20/60</f>
-        <v>0.23546389333333334</v>
+        <v>0.39243982666666671</v>
       </c>
       <c r="K20" s="3">
         <f t="shared" si="36"/>
-        <v>3.9243982222222223E-3</v>
-      </c>
-    </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.3">
+        <v>6.5406637777777783E-3</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A21" s="2">
         <v>21</v>
       </c>
@@ -1456,30 +1482,34 @@
       <c r="D21" s="1">
         <v>47323624</v>
       </c>
-      <c r="E21" s="1"/>
-      <c r="F21" s="1"/>
+      <c r="E21" s="1">
+        <v>47323624</v>
+      </c>
+      <c r="F21" s="1">
+        <v>47323624</v>
+      </c>
       <c r="G21" s="1">
         <f t="shared" si="0"/>
-        <v>28394182.399999999</v>
+        <v>47323632</v>
       </c>
       <c r="H21" s="1">
         <f t="shared" ref="H21:I21" si="37">G21/1000</f>
-        <v>28394.182399999998</v>
-      </c>
-      <c r="I21" s="1">
+        <v>47323.631999999998</v>
+      </c>
+      <c r="I21" s="16">
         <f t="shared" si="37"/>
-        <v>28.394182399999998</v>
+        <v>47.323631999999996</v>
       </c>
       <c r="J21" s="1">
         <f t="shared" ref="J21:K21" si="38">I21/60</f>
-        <v>0.47323637333333329</v>
+        <v>0.78872719999999996</v>
       </c>
       <c r="K21" s="3">
         <f t="shared" si="38"/>
-        <v>7.8872728888888886E-3</v>
-      </c>
-    </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.3">
+        <v>1.3145453333333333E-2</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A22" s="2">
         <v>22</v>
       </c>
@@ -1492,30 +1522,34 @@
       <c r="D22" s="1">
         <v>94878091</v>
       </c>
-      <c r="E22" s="1"/>
-      <c r="F22" s="1"/>
+      <c r="E22" s="1">
+        <v>94878091</v>
+      </c>
+      <c r="F22" s="1">
+        <v>94878091</v>
+      </c>
       <c r="G22" s="1">
         <f t="shared" si="0"/>
-        <v>56926854.399999999</v>
+        <v>94878090.799999997</v>
       </c>
       <c r="H22" s="1">
         <f t="shared" ref="H22:I22" si="39">G22/1000</f>
-        <v>56926.854399999997</v>
-      </c>
-      <c r="I22" s="1">
+        <v>94878.090799999991</v>
+      </c>
+      <c r="I22" s="16">
         <f t="shared" si="39"/>
-        <v>56.926854399999996</v>
+        <v>94.878090799999995</v>
       </c>
       <c r="J22" s="1">
         <f t="shared" ref="J22:K22" si="40">I22/60</f>
-        <v>0.94878090666666659</v>
+        <v>1.5813015133333332</v>
       </c>
       <c r="K22" s="3">
         <f t="shared" si="40"/>
-        <v>1.581301511111111E-2</v>
-      </c>
-    </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.3">
+        <v>2.635502522222222E-2</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A23" s="2">
         <v>23</v>
       </c>
@@ -1528,30 +1562,34 @@
       <c r="D23" s="1">
         <v>189987025</v>
       </c>
-      <c r="E23" s="1"/>
-      <c r="F23" s="1"/>
+      <c r="E23" s="1">
+        <v>189987025</v>
+      </c>
+      <c r="F23" s="1">
+        <v>189987026</v>
+      </c>
       <c r="G23" s="1">
         <f t="shared" si="0"/>
-        <v>113992215</v>
+        <v>189987025.19999999</v>
       </c>
       <c r="H23" s="1">
         <f t="shared" ref="H23:I23" si="41">G23/1000</f>
-        <v>113992.215</v>
-      </c>
-      <c r="I23" s="1">
+        <v>189987.02519999997</v>
+      </c>
+      <c r="I23" s="16">
         <f t="shared" si="41"/>
-        <v>113.992215</v>
+        <v>189.98702519999998</v>
       </c>
       <c r="J23" s="1">
         <f t="shared" ref="J23:K23" si="42">I23/60</f>
-        <v>1.89987025</v>
+        <v>3.1664504199999994</v>
       </c>
       <c r="K23" s="3">
         <f t="shared" si="42"/>
-        <v>3.166450416666667E-2</v>
-      </c>
-    </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.3">
+        <v>5.277417366666666E-2</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A24" s="2">
         <v>24</v>
       </c>
@@ -1562,269 +1600,294 @@
         <v>380204893</v>
       </c>
       <c r="D24" s="1">
-        <v>3802048892</v>
-      </c>
-      <c r="E24" s="1"/>
-      <c r="F24" s="1"/>
+        <v>380204892</v>
+      </c>
+      <c r="E24" s="1">
+        <v>380204893</v>
+      </c>
+      <c r="F24" s="1">
+        <v>380204894</v>
+      </c>
       <c r="G24" s="1">
         <f t="shared" si="0"/>
-        <v>912491735.39999998</v>
+        <v>380204892.80000001</v>
       </c>
       <c r="H24" s="1">
         <f t="shared" ref="H24:I24" si="43">G24/1000</f>
-        <v>912491.73540000001</v>
-      </c>
-      <c r="I24" s="1">
+        <v>380204.89280000003</v>
+      </c>
+      <c r="I24" s="16">
         <f t="shared" si="43"/>
-        <v>912.49173540000004</v>
+        <v>380.20489280000004</v>
       </c>
       <c r="J24" s="1">
         <f t="shared" ref="J24:K24" si="44">I24/60</f>
-        <v>15.208195590000001</v>
+        <v>6.3367482133333342</v>
       </c>
       <c r="K24" s="3">
         <f t="shared" si="44"/>
-        <v>0.2534699265</v>
-      </c>
-    </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.3">
+        <v>0.10561247022222224</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A25" s="2">
         <v>25</v>
       </c>
-      <c r="B25" s="1"/>
+      <c r="B25" s="1">
+        <v>760636942</v>
+      </c>
       <c r="C25" s="1"/>
       <c r="D25" s="1"/>
       <c r="E25" s="1"/>
       <c r="F25" s="1"/>
       <c r="G25" s="1">
         <f>SUM(B25:F25)</f>
-        <v>0</v>
+        <v>760636942</v>
       </c>
       <c r="H25" s="1">
         <f t="shared" ref="H25:I25" si="45">G25/1000</f>
-        <v>0</v>
-      </c>
-      <c r="I25" s="1">
+        <v>760636.94200000004</v>
+      </c>
+      <c r="I25" s="16">
         <f t="shared" si="45"/>
-        <v>0</v>
+        <v>760.63694200000009</v>
       </c>
       <c r="J25" s="1">
         <f t="shared" ref="J25:K25" si="46">I25/60</f>
-        <v>0</v>
+        <v>12.677282366666669</v>
       </c>
       <c r="K25" s="3">
         <f t="shared" si="46"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.3">
+        <v>0.21128803944444446</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A26" s="2">
         <v>26</v>
       </c>
-      <c r="B26" s="1"/>
+      <c r="B26" s="14">
+        <v>1521511257</v>
+      </c>
       <c r="C26" s="1"/>
       <c r="D26" s="1"/>
       <c r="E26" s="1"/>
       <c r="F26" s="1"/>
       <c r="G26" s="1">
         <f t="shared" ref="G26:G32" si="47">SUM(B26:F26)</f>
-        <v>0</v>
+        <v>1521511257</v>
       </c>
       <c r="H26" s="1">
         <f t="shared" ref="H26:I26" si="48">G26/1000</f>
-        <v>0</v>
-      </c>
-      <c r="I26" s="1">
+        <v>1521511.257</v>
+      </c>
+      <c r="I26" s="16">
         <f t="shared" si="48"/>
-        <v>0</v>
+        <v>1521.5112569999999</v>
       </c>
       <c r="J26" s="1">
         <f t="shared" ref="J26:K26" si="49">I26/60</f>
-        <v>0</v>
+        <v>25.358520949999999</v>
       </c>
       <c r="K26" s="3">
         <f t="shared" si="49"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="27" spans="1:12" x14ac:dyDescent="0.3">
+        <v>0.42264201583333333</v>
+      </c>
+    </row>
+    <row r="27" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A27" s="2">
         <v>27</v>
       </c>
-      <c r="B27" s="1"/>
+      <c r="B27" s="1">
+        <v>3043253279</v>
+      </c>
       <c r="C27" s="1"/>
       <c r="D27" s="1"/>
       <c r="E27" s="1"/>
       <c r="F27" s="1"/>
       <c r="G27" s="1">
         <f t="shared" si="47"/>
-        <v>0</v>
+        <v>3043253279</v>
       </c>
       <c r="H27" s="1">
         <f t="shared" ref="H27:I27" si="50">G27/1000</f>
-        <v>0</v>
-      </c>
-      <c r="I27" s="1">
+        <v>3043253.2790000001</v>
+      </c>
+      <c r="I27" s="16">
         <f t="shared" si="50"/>
-        <v>0</v>
+        <v>3043.253279</v>
       </c>
       <c r="J27" s="1">
         <f t="shared" ref="J27:K27" si="51">I27/60</f>
-        <v>0</v>
+        <v>50.720887983333334</v>
       </c>
       <c r="K27" s="3">
         <f t="shared" si="51"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="28" spans="1:12" x14ac:dyDescent="0.3">
+        <v>0.84534813305555556</v>
+      </c>
+    </row>
+    <row r="28" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A28" s="2">
         <v>28</v>
       </c>
-      <c r="B28" s="1"/>
+      <c r="B28" s="1">
+        <f>B27*2+118356</f>
+        <v>6086624914</v>
+      </c>
       <c r="C28" s="1"/>
       <c r="D28" s="1"/>
       <c r="E28" s="1"/>
       <c r="F28" s="1"/>
       <c r="G28" s="1">
         <f t="shared" si="47"/>
-        <v>0</v>
+        <v>6086624914</v>
       </c>
       <c r="H28" s="1">
         <f t="shared" ref="H28:I28" si="52">G28/1000</f>
-        <v>0</v>
-      </c>
-      <c r="I28" s="1">
+        <v>6086624.9139999999</v>
+      </c>
+      <c r="I28" s="16">
         <f t="shared" si="52"/>
-        <v>0</v>
+        <v>6086.624914</v>
       </c>
       <c r="J28" s="1">
         <f t="shared" ref="J28:K28" si="53">I28/60</f>
-        <v>0</v>
+        <v>101.44374856666667</v>
       </c>
       <c r="K28" s="3">
         <f t="shared" si="53"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="29" spans="1:12" x14ac:dyDescent="0.3">
+        <v>1.6907291427777777</v>
+      </c>
+    </row>
+    <row r="29" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A29" s="2">
         <v>29</v>
       </c>
-      <c r="B29" s="1"/>
+      <c r="B29" s="1">
+        <f t="shared" ref="B29:B32" si="54">B28*2+118356</f>
+        <v>12173368184</v>
+      </c>
       <c r="C29" s="1"/>
       <c r="D29" s="1"/>
       <c r="E29" s="1"/>
       <c r="F29" s="1"/>
       <c r="G29" s="1">
         <f t="shared" si="47"/>
-        <v>0</v>
+        <v>12173368184</v>
       </c>
       <c r="H29" s="1">
-        <f t="shared" ref="H29:I29" si="54">G29/1000</f>
-        <v>0</v>
-      </c>
-      <c r="I29" s="1">
-        <f t="shared" si="54"/>
-        <v>0</v>
+        <f t="shared" ref="H29:I29" si="55">G29/1000</f>
+        <v>12173368.184</v>
+      </c>
+      <c r="I29" s="16">
+        <f t="shared" si="55"/>
+        <v>12173.368184000001</v>
       </c>
       <c r="J29" s="1">
-        <f t="shared" ref="J29:K29" si="55">I29/60</f>
-        <v>0</v>
+        <f t="shared" ref="J29:K29" si="56">I29/60</f>
+        <v>202.88946973333336</v>
       </c>
       <c r="K29" s="3">
-        <f t="shared" si="55"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="30" spans="1:12" x14ac:dyDescent="0.3">
+        <f t="shared" si="56"/>
+        <v>3.3814911622222228</v>
+      </c>
+    </row>
+    <row r="30" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A30" s="2">
         <v>30</v>
       </c>
-      <c r="B30" s="1"/>
+      <c r="B30" s="1">
+        <f t="shared" si="54"/>
+        <v>24346854724</v>
+      </c>
       <c r="C30" s="1"/>
       <c r="D30" s="1"/>
       <c r="E30" s="1"/>
       <c r="F30" s="1"/>
       <c r="G30" s="1">
         <f t="shared" si="47"/>
-        <v>0</v>
+        <v>24346854724</v>
       </c>
       <c r="H30" s="1">
-        <f t="shared" ref="H30:I30" si="56">G30/1000</f>
-        <v>0</v>
-      </c>
-      <c r="I30" s="1">
-        <f t="shared" si="56"/>
-        <v>0</v>
+        <f t="shared" ref="H30:I30" si="57">G30/1000</f>
+        <v>24346854.723999999</v>
+      </c>
+      <c r="I30" s="16">
+        <f t="shared" si="57"/>
+        <v>24346.854724000001</v>
       </c>
       <c r="J30" s="1">
-        <f t="shared" ref="J30:K30" si="57">I30/60</f>
-        <v>0</v>
+        <f t="shared" ref="J30:K30" si="58">I30/60</f>
+        <v>405.7809120666667</v>
       </c>
       <c r="K30" s="3">
-        <f t="shared" si="57"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="31" spans="1:12" x14ac:dyDescent="0.3">
+        <f t="shared" si="58"/>
+        <v>6.763015201111112</v>
+      </c>
+    </row>
+    <row r="31" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A31" s="2">
         <v>31</v>
       </c>
-      <c r="B31" s="1"/>
+      <c r="B31" s="1">
+        <f t="shared" si="54"/>
+        <v>48693827804</v>
+      </c>
       <c r="C31" s="1"/>
       <c r="D31" s="1"/>
       <c r="E31" s="1"/>
       <c r="F31" s="1"/>
       <c r="G31" s="1">
         <f t="shared" si="47"/>
-        <v>0</v>
+        <v>48693827804</v>
       </c>
       <c r="H31" s="1">
-        <f t="shared" ref="H31:I31" si="58">G31/1000</f>
-        <v>0</v>
-      </c>
-      <c r="I31" s="1">
-        <f t="shared" si="58"/>
-        <v>0</v>
+        <f t="shared" ref="H31:I31" si="59">G31/1000</f>
+        <v>48693827.803999998</v>
+      </c>
+      <c r="I31" s="16">
+        <f t="shared" si="59"/>
+        <v>48693.827804</v>
       </c>
       <c r="J31" s="1">
-        <f t="shared" ref="J31:K31" si="59">I31/60</f>
-        <v>0</v>
+        <f t="shared" ref="J31:K31" si="60">I31/60</f>
+        <v>811.56379673333333</v>
       </c>
       <c r="K31" s="3">
-        <f t="shared" si="59"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="32" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+        <f t="shared" si="60"/>
+        <v>13.526063278888889</v>
+      </c>
+    </row>
+    <row r="32" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A32" s="4">
         <v>32</v>
       </c>
-      <c r="B32" s="5"/>
+      <c r="B32" s="1">
+        <f t="shared" si="54"/>
+        <v>97387773964</v>
+      </c>
       <c r="C32" s="5"/>
       <c r="D32" s="5"/>
       <c r="E32" s="5"/>
       <c r="F32" s="5"/>
       <c r="G32" s="5">
         <f t="shared" si="47"/>
-        <v>0</v>
+        <v>97387773964</v>
       </c>
       <c r="H32" s="5">
-        <f t="shared" ref="H32:I32" si="60">G32/1000</f>
-        <v>0</v>
-      </c>
-      <c r="I32" s="5">
-        <f t="shared" si="60"/>
-        <v>0</v>
+        <f t="shared" ref="H32:I32" si="61">G32/1000</f>
+        <v>97387773.964000002</v>
+      </c>
+      <c r="I32" s="17">
+        <f t="shared" si="61"/>
+        <v>97387.773964000007</v>
       </c>
       <c r="J32" s="5">
-        <f t="shared" ref="J32:K32" si="61">I32/60</f>
-        <v>0</v>
+        <f t="shared" ref="J32:K32" si="62">I32/60</f>
+        <v>1623.1295660666667</v>
       </c>
       <c r="K32" s="6">
-        <f t="shared" si="61"/>
-        <v>0</v>
+        <f t="shared" si="62"/>
+        <v>27.052159434444444</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Implemented code seemingly capable of measuring at 6 microphones despite them not being TDM compatible. NOT in realtime though, but close
</commit_message>
<xml_diff>
--- a/Project/Kode/MLSGeneratorAverageTimes.xlsx
+++ b/Project/Kode/MLSGeneratorAverageTimes.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Christian Lykke\Documents\Skole\Aalborg Universitet\ESD6\Project\Kode\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2049A843-0F06-447A-ACD8-B95C08D5D270}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{05B263F7-20B4-4E34-8D90-5334CBDA6226}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="19200" yWindow="-21600" windowWidth="19200" windowHeight="21000" xr2:uid="{77718FEC-CCAD-4B45-B589-CCDFD0FA239E}"/>
+    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12552" xr2:uid="{77718FEC-CCAD-4B45-B589-CCDFD0FA239E}"/>
   </bookViews>
   <sheets>
     <sheet name="Ark1" sheetId="1" r:id="rId1"/>
@@ -299,7 +299,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -314,12 +314,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -654,1238 +656,1239 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6CEF9135-1CC1-4529-B399-B9FADBA0A2F0}">
-  <dimension ref="A1:L32"/>
+  <dimension ref="B1:M33"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L1" sqref="L1:L22"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="N19" sqref="N19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="9.33203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12" bestFit="1" customWidth="1"/>
-    <col min="4" max="6" width="10" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="11" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="14" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="12.33203125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="18.109375" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="15.77734375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12" bestFit="1" customWidth="1"/>
+    <col min="5" max="7" width="10" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="14" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="12.33203125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="18.109375" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="15.77734375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="10" t="s">
+    <row r="1" spans="2:13" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="2" spans="2:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B2" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="11" t="s">
+      <c r="C2" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="11" t="s">
+      <c r="D2" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="11" t="s">
+      <c r="E2" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="11" t="s">
+      <c r="F2" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="11" t="s">
+      <c r="G2" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="11" t="s">
+      <c r="H2" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="11" t="s">
+      <c r="I2" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="11" t="s">
+      <c r="J2" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="11" t="s">
+      <c r="K2" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="12" t="s">
+      <c r="L2" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="13"/>
-    </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A2" s="7">
+      <c r="M2" s="13"/>
+    </row>
+    <row r="3" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="B3" s="7">
         <v>2</v>
       </c>
-      <c r="B2" s="8">
+      <c r="C3" s="8">
         <v>1</v>
       </c>
-      <c r="C2" s="8">
+      <c r="D3" s="8">
         <v>1</v>
       </c>
-      <c r="D2" s="8">
+      <c r="E3" s="8">
         <v>1</v>
       </c>
-      <c r="E2" s="8">
+      <c r="F3" s="8">
         <v>1</v>
       </c>
-      <c r="F2" s="8">
+      <c r="G3" s="8">
         <v>1</v>
       </c>
-      <c r="G2" s="8">
-        <f>SUM(B2:F2)/5</f>
+      <c r="H3" s="8">
+        <f>SUM(C3:G3)/5</f>
         <v>1</v>
       </c>
-      <c r="H2" s="8">
-        <f>G2/1000</f>
+      <c r="I3" s="8">
+        <f>H3/1000</f>
         <v>1E-3</v>
       </c>
-      <c r="I2" s="15">
-        <f>H2/1000</f>
+      <c r="J3" s="14">
+        <f>I3/1000</f>
         <v>9.9999999999999995E-7</v>
       </c>
-      <c r="J2" s="8">
-        <f>I2/60</f>
+      <c r="K3" s="8">
+        <f>J3/60</f>
         <v>1.6666666666666667E-8</v>
       </c>
-      <c r="K2" s="9">
-        <f>J2/60</f>
+      <c r="L3" s="9">
+        <f>K3/60</f>
         <v>2.7777777777777777E-10</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A3" s="2">
+    <row r="4" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="B4" s="2">
         <v>3</v>
       </c>
-      <c r="B3" s="1">
+      <c r="C4" s="1">
         <v>2</v>
       </c>
-      <c r="C3" s="1">
+      <c r="D4" s="1">
         <v>2</v>
       </c>
-      <c r="D3" s="1">
+      <c r="E4" s="1">
         <v>2</v>
       </c>
-      <c r="E3" s="1">
+      <c r="F4" s="1">
         <v>1</v>
       </c>
-      <c r="F3" s="1">
+      <c r="G4" s="1">
         <v>1</v>
       </c>
-      <c r="G3" s="1">
-        <f t="shared" ref="G3:G24" si="0">SUM(B3:F3)/5</f>
+      <c r="H4" s="1">
+        <f t="shared" ref="H4:H25" si="0">SUM(C4:G4)/5</f>
         <v>1.6</v>
       </c>
-      <c r="H3" s="1">
-        <f t="shared" ref="H3:I3" si="1">G3/1000</f>
+      <c r="I4" s="1">
+        <f t="shared" ref="I4:J4" si="1">H4/1000</f>
         <v>1.6000000000000001E-3</v>
       </c>
-      <c r="I3" s="16">
+      <c r="J4" s="15">
         <f t="shared" si="1"/>
         <v>1.6000000000000001E-6</v>
       </c>
-      <c r="J3" s="1">
-        <f t="shared" ref="J3:K3" si="2">I3/60</f>
+      <c r="K4" s="1">
+        <f t="shared" ref="K4:L4" si="2">J4/60</f>
         <v>2.6666666666666671E-8</v>
       </c>
-      <c r="K3" s="3">
+      <c r="L4" s="3">
         <f t="shared" si="2"/>
         <v>4.4444444444444453E-10</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A4" s="2">
+    <row r="5" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="B5" s="2">
         <v>4</v>
       </c>
-      <c r="B4" s="1">
+      <c r="C5" s="1">
         <v>2</v>
       </c>
-      <c r="C4" s="1">
+      <c r="D5" s="1">
         <v>2</v>
       </c>
-      <c r="D4" s="1">
+      <c r="E5" s="1">
         <v>2</v>
       </c>
-      <c r="E4" s="1">
+      <c r="F5" s="1">
         <v>1</v>
       </c>
-      <c r="F4" s="1">
+      <c r="G5" s="1">
         <v>1</v>
       </c>
-      <c r="G4" s="1">
+      <c r="H5" s="1">
         <f t="shared" si="0"/>
         <v>1.6</v>
       </c>
-      <c r="H4" s="1">
-        <f t="shared" ref="H4:I4" si="3">G4/1000</f>
+      <c r="I5" s="1">
+        <f t="shared" ref="I5:J5" si="3">H5/1000</f>
         <v>1.6000000000000001E-3</v>
       </c>
-      <c r="I4" s="16">
+      <c r="J5" s="15">
         <f t="shared" si="3"/>
         <v>1.6000000000000001E-6</v>
       </c>
-      <c r="J4" s="1">
-        <f t="shared" ref="J4:K4" si="4">I4/60</f>
+      <c r="K5" s="1">
+        <f t="shared" ref="K5:L5" si="4">J5/60</f>
         <v>2.6666666666666671E-8</v>
       </c>
-      <c r="K4" s="3">
+      <c r="L5" s="3">
         <f t="shared" si="4"/>
         <v>4.4444444444444453E-10</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A5" s="2">
+    <row r="6" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="B6" s="2">
         <v>5</v>
       </c>
-      <c r="B5" s="1">
+      <c r="C6" s="1">
         <v>3</v>
       </c>
-      <c r="C5" s="1">
+      <c r="D6" s="1">
         <v>3</v>
       </c>
-      <c r="D5" s="1">
+      <c r="E6" s="1">
         <v>3</v>
       </c>
-      <c r="E5" s="1">
+      <c r="F6" s="1">
         <v>2</v>
       </c>
-      <c r="F5" s="1">
+      <c r="G6" s="1">
         <v>2</v>
       </c>
-      <c r="G5" s="1">
+      <c r="H6" s="1">
         <f t="shared" si="0"/>
         <v>2.6</v>
       </c>
-      <c r="H5" s="1">
-        <f t="shared" ref="H5:I5" si="5">G5/1000</f>
+      <c r="I6" s="1">
+        <f t="shared" ref="I6:J6" si="5">H6/1000</f>
         <v>2.5999999999999999E-3</v>
       </c>
-      <c r="I5" s="16">
+      <c r="J6" s="15">
         <f t="shared" si="5"/>
         <v>2.5999999999999997E-6</v>
       </c>
-      <c r="J5" s="1">
-        <f t="shared" ref="J5:K5" si="6">I5/60</f>
+      <c r="K6" s="1">
+        <f t="shared" ref="K6:L6" si="6">J6/60</f>
         <v>4.3333333333333331E-8</v>
       </c>
-      <c r="K5" s="3">
+      <c r="L6" s="3">
         <f t="shared" si="6"/>
         <v>7.2222222222222214E-10</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A6" s="2">
+    <row r="7" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="B7" s="2">
         <v>6</v>
       </c>
-      <c r="B6" s="1">
+      <c r="C7" s="1">
         <v>5</v>
       </c>
-      <c r="C6" s="1">
+      <c r="D7" s="1">
         <v>5</v>
       </c>
-      <c r="D6" s="1">
+      <c r="E7" s="1">
         <v>5</v>
       </c>
-      <c r="E6" s="1">
+      <c r="F7" s="1">
         <v>4</v>
       </c>
-      <c r="F6" s="1">
+      <c r="G7" s="1">
         <v>4</v>
       </c>
-      <c r="G6" s="1">
+      <c r="H7" s="1">
         <f t="shared" si="0"/>
         <v>4.5999999999999996</v>
       </c>
-      <c r="H6" s="1">
-        <f t="shared" ref="H6:I6" si="7">G6/1000</f>
+      <c r="I7" s="1">
+        <f t="shared" ref="I7:J7" si="7">H7/1000</f>
         <v>4.5999999999999999E-3</v>
       </c>
-      <c r="I6" s="16">
+      <c r="J7" s="15">
         <f t="shared" si="7"/>
         <v>4.6E-6</v>
       </c>
-      <c r="J6" s="1">
-        <f t="shared" ref="J6:K6" si="8">I6/60</f>
+      <c r="K7" s="1">
+        <f t="shared" ref="K7:L7" si="8">J7/60</f>
         <v>7.6666666666666665E-8</v>
       </c>
-      <c r="K6" s="3">
+      <c r="L7" s="3">
         <f t="shared" si="8"/>
         <v>1.2777777777777778E-9</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A7" s="2">
+    <row r="8" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="B8" s="2">
         <v>7</v>
       </c>
-      <c r="B7" s="1">
+      <c r="C8" s="1">
         <v>8</v>
       </c>
-      <c r="C7" s="1">
+      <c r="D8" s="1">
         <v>8</v>
       </c>
-      <c r="D7" s="1">
+      <c r="E8" s="1">
         <v>10</v>
       </c>
-      <c r="E7" s="1">
+      <c r="F8" s="1">
         <v>8</v>
       </c>
-      <c r="F7" s="1">
+      <c r="G8" s="1">
         <v>8</v>
       </c>
-      <c r="G7" s="1">
+      <c r="H8" s="1">
         <f t="shared" si="0"/>
         <v>8.4</v>
       </c>
-      <c r="H7" s="1">
-        <f t="shared" ref="H7:I7" si="9">G7/1000</f>
+      <c r="I8" s="1">
+        <f t="shared" ref="I8:J8" si="9">H8/1000</f>
         <v>8.4000000000000012E-3</v>
       </c>
-      <c r="I7" s="16">
+      <c r="J8" s="15">
         <f t="shared" si="9"/>
         <v>8.4000000000000009E-6</v>
       </c>
-      <c r="J7" s="1">
-        <f t="shared" ref="J7:K7" si="10">I7/60</f>
+      <c r="K8" s="1">
+        <f t="shared" ref="K8:L8" si="10">J8/60</f>
         <v>1.4000000000000001E-7</v>
       </c>
-      <c r="K7" s="3">
+      <c r="L8" s="3">
         <f t="shared" si="10"/>
         <v>2.3333333333333335E-9</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A8" s="2">
+    <row r="9" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="B9" s="2">
         <v>8</v>
       </c>
-      <c r="B8" s="1">
+      <c r="C9" s="1">
         <v>15</v>
       </c>
-      <c r="C8" s="1">
+      <c r="D9" s="1">
         <v>15</v>
       </c>
-      <c r="D8" s="1">
+      <c r="E9" s="1">
         <v>15</v>
       </c>
-      <c r="E8" s="1">
+      <c r="F9" s="1">
         <v>14</v>
       </c>
-      <c r="F8" s="1">
+      <c r="G9" s="1">
         <v>14</v>
       </c>
-      <c r="G8" s="1">
+      <c r="H9" s="1">
         <f t="shared" si="0"/>
         <v>14.6</v>
       </c>
-      <c r="H8" s="1">
-        <f t="shared" ref="H8:I8" si="11">G8/1000</f>
+      <c r="I9" s="1">
+        <f t="shared" ref="I9:J9" si="11">H9/1000</f>
         <v>1.46E-2</v>
       </c>
-      <c r="I8" s="16">
+      <c r="J9" s="15">
         <f t="shared" si="11"/>
         <v>1.4600000000000001E-5</v>
       </c>
-      <c r="J8" s="1">
-        <f t="shared" ref="J8:K8" si="12">I8/60</f>
+      <c r="K9" s="1">
+        <f t="shared" ref="K9:L9" si="12">J9/60</f>
         <v>2.4333333333333337E-7</v>
       </c>
-      <c r="K8" s="3">
+      <c r="L9" s="3">
         <f t="shared" si="12"/>
         <v>4.0555555555555558E-9</v>
       </c>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A9" s="2">
+    <row r="10" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="B10" s="2">
         <v>9</v>
       </c>
-      <c r="B9" s="1">
+      <c r="C10" s="1">
         <v>28</v>
       </c>
-      <c r="C9" s="1">
+      <c r="D10" s="1">
         <v>28</v>
       </c>
-      <c r="D9" s="1">
+      <c r="E10" s="1">
         <v>28</v>
       </c>
-      <c r="E9" s="1">
+      <c r="F10" s="1">
         <v>27</v>
       </c>
-      <c r="F9" s="1">
+      <c r="G10" s="1">
         <v>27</v>
       </c>
-      <c r="G9" s="1">
+      <c r="H10" s="1">
         <f t="shared" si="0"/>
         <v>27.6</v>
       </c>
-      <c r="H9" s="1">
-        <f t="shared" ref="H9:I9" si="13">G9/1000</f>
+      <c r="I10" s="1">
+        <f t="shared" ref="I10:J10" si="13">H10/1000</f>
         <v>2.7600000000000003E-2</v>
       </c>
-      <c r="I9" s="16">
+      <c r="J10" s="15">
         <f t="shared" si="13"/>
         <v>2.7600000000000003E-5</v>
       </c>
-      <c r="J9" s="1">
-        <f t="shared" ref="J9:K9" si="14">I9/60</f>
+      <c r="K10" s="1">
+        <f t="shared" ref="K10:L10" si="14">J10/60</f>
         <v>4.6000000000000004E-7</v>
       </c>
-      <c r="K9" s="3">
+      <c r="L10" s="3">
         <f t="shared" si="14"/>
         <v>7.6666666666666675E-9</v>
       </c>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A10" s="2">
+    <row r="11" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="B11" s="2">
         <v>10</v>
       </c>
-      <c r="B10" s="1">
+      <c r="C11" s="1">
         <v>53</v>
       </c>
-      <c r="C10" s="1">
+      <c r="D11" s="1">
         <v>53</v>
       </c>
-      <c r="D10" s="1">
+      <c r="E11" s="1">
         <v>53</v>
       </c>
-      <c r="E10" s="1">
+      <c r="F11" s="1">
         <v>53</v>
       </c>
-      <c r="F10" s="1">
+      <c r="G11" s="1">
         <v>53</v>
       </c>
-      <c r="G10" s="1">
+      <c r="H11" s="1">
         <f t="shared" si="0"/>
         <v>53</v>
       </c>
-      <c r="H10" s="1">
-        <f t="shared" ref="H10:I10" si="15">G10/1000</f>
+      <c r="I11" s="1">
+        <f t="shared" ref="I11:J11" si="15">H11/1000</f>
         <v>5.2999999999999999E-2</v>
       </c>
-      <c r="I10" s="16">
+      <c r="J11" s="15">
         <f t="shared" si="15"/>
         <v>5.3000000000000001E-5</v>
       </c>
-      <c r="J10" s="1">
-        <f t="shared" ref="J10:K10" si="16">I10/60</f>
+      <c r="K11" s="1">
+        <f t="shared" ref="K11:L11" si="16">J11/60</f>
         <v>8.8333333333333338E-7</v>
       </c>
-      <c r="K10" s="3">
+      <c r="L11" s="3">
         <f t="shared" si="16"/>
         <v>1.4722222222222223E-8</v>
       </c>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A11" s="2">
+    <row r="12" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="B12" s="2">
         <v>11</v>
       </c>
-      <c r="B11" s="1">
+      <c r="C12" s="1">
         <v>106</v>
       </c>
-      <c r="C11" s="1">
+      <c r="D12" s="1">
         <v>108</v>
       </c>
-      <c r="D11" s="1">
+      <c r="E12" s="1">
         <v>106</v>
       </c>
-      <c r="E11" s="1">
+      <c r="F12" s="1">
         <v>106</v>
       </c>
-      <c r="F11" s="1">
+      <c r="G12" s="1">
         <v>106</v>
       </c>
-      <c r="G11" s="1">
+      <c r="H12" s="1">
         <f t="shared" si="0"/>
         <v>106.4</v>
       </c>
-      <c r="H11" s="1">
-        <f t="shared" ref="H11:I11" si="17">G11/1000</f>
+      <c r="I12" s="1">
+        <f t="shared" ref="I12:J12" si="17">H12/1000</f>
         <v>0.10640000000000001</v>
       </c>
-      <c r="I11" s="16">
+      <c r="J12" s="15">
         <f t="shared" si="17"/>
         <v>1.0640000000000001E-4</v>
       </c>
-      <c r="J11" s="1">
-        <f t="shared" ref="J11:K11" si="18">I11/60</f>
+      <c r="K12" s="1">
+        <f t="shared" ref="K12:L12" si="18">J12/60</f>
         <v>1.7733333333333334E-6</v>
       </c>
-      <c r="K11" s="3">
+      <c r="L12" s="3">
         <f t="shared" si="18"/>
         <v>2.9555555555555557E-8</v>
       </c>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A12" s="2">
+    <row r="13" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="B13" s="2">
         <v>12</v>
       </c>
-      <c r="B12" s="1">
+      <c r="C13" s="1">
         <v>208</v>
       </c>
-      <c r="C12" s="1">
+      <c r="D13" s="1">
         <v>209</v>
       </c>
-      <c r="D12" s="1">
+      <c r="E13" s="1">
         <v>208</v>
       </c>
-      <c r="E12" s="1">
+      <c r="F13" s="1">
         <v>208</v>
       </c>
-      <c r="F12" s="1">
+      <c r="G13" s="1">
         <v>208</v>
       </c>
-      <c r="G12" s="1">
+      <c r="H13" s="1">
         <f t="shared" si="0"/>
         <v>208.2</v>
       </c>
-      <c r="H12" s="1">
-        <f t="shared" ref="H12:I12" si="19">G12/1000</f>
+      <c r="I13" s="1">
+        <f t="shared" ref="I13:J13" si="19">H13/1000</f>
         <v>0.2082</v>
       </c>
-      <c r="I12" s="16">
+      <c r="J13" s="15">
         <f t="shared" si="19"/>
         <v>2.0819999999999999E-4</v>
       </c>
-      <c r="J12" s="1">
-        <f t="shared" ref="J12:K12" si="20">I12/60</f>
+      <c r="K13" s="1">
+        <f t="shared" ref="K13:L13" si="20">J13/60</f>
         <v>3.4699999999999998E-6</v>
       </c>
-      <c r="K12" s="3">
+      <c r="L13" s="3">
         <f t="shared" si="20"/>
         <v>5.7833333333333328E-8</v>
       </c>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A13" s="2">
+    <row r="14" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="B14" s="2">
         <v>13</v>
       </c>
-      <c r="B13" s="1">
+      <c r="C14" s="1">
         <v>419</v>
       </c>
-      <c r="C13" s="1">
+      <c r="D14" s="1">
         <v>418</v>
       </c>
-      <c r="D13" s="1">
+      <c r="E14" s="1">
         <v>418</v>
       </c>
-      <c r="E13" s="1">
+      <c r="F14" s="1">
         <v>419</v>
       </c>
-      <c r="F13" s="1">
+      <c r="G14" s="1">
         <v>418</v>
       </c>
-      <c r="G13" s="1">
+      <c r="H14" s="1">
         <f t="shared" si="0"/>
         <v>418.4</v>
       </c>
-      <c r="H13" s="1">
-        <f t="shared" ref="H13:I13" si="21">G13/1000</f>
+      <c r="I14" s="1">
+        <f t="shared" ref="I14:J14" si="21">H14/1000</f>
         <v>0.41839999999999999</v>
       </c>
-      <c r="I13" s="16">
+      <c r="J14" s="15">
         <f t="shared" si="21"/>
         <v>4.1839999999999998E-4</v>
       </c>
-      <c r="J13" s="1">
-        <f t="shared" ref="J13:K13" si="22">I13/60</f>
+      <c r="K14" s="1">
+        <f t="shared" ref="K14:L14" si="22">J14/60</f>
         <v>6.9733333333333332E-6</v>
       </c>
-      <c r="K13" s="3">
+      <c r="L14" s="3">
         <f t="shared" si="22"/>
         <v>1.1622222222222222E-7</v>
       </c>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A14" s="2">
+    <row r="15" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="B15" s="2">
         <v>14</v>
       </c>
-      <c r="B14" s="1">
+      <c r="C15" s="1">
         <v>140682</v>
       </c>
-      <c r="C14" s="1">
+      <c r="D15" s="1">
         <v>139850</v>
       </c>
-      <c r="D14" s="1">
+      <c r="E15" s="1">
         <v>142186</v>
       </c>
-      <c r="E14" s="1">
+      <c r="F15" s="1">
         <v>141986</v>
       </c>
-      <c r="F14" s="1">
+      <c r="G15" s="1">
         <v>141048</v>
       </c>
-      <c r="G14" s="1">
+      <c r="H15" s="1">
         <f t="shared" si="0"/>
         <v>141150.39999999999</v>
       </c>
-      <c r="H14" s="1">
-        <f t="shared" ref="H14:I14" si="23">G14/1000</f>
+      <c r="I15" s="1">
+        <f t="shared" ref="I15:J15" si="23">H15/1000</f>
         <v>141.15039999999999</v>
       </c>
-      <c r="I14" s="16">
+      <c r="J15" s="15">
         <f t="shared" si="23"/>
         <v>0.14115039999999998</v>
       </c>
-      <c r="J14" s="1">
-        <f t="shared" ref="J14:K14" si="24">I14/60</f>
+      <c r="K15" s="1">
+        <f t="shared" ref="K15:L15" si="24">J15/60</f>
         <v>2.3525066666666662E-3</v>
       </c>
-      <c r="K14" s="3">
+      <c r="L15" s="3">
         <f t="shared" si="24"/>
         <v>3.9208444444444438E-5</v>
       </c>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A15" s="2">
+    <row r="16" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="B16" s="2">
         <v>15</v>
       </c>
-      <c r="B15" s="1">
+      <c r="C16" s="1">
         <v>512195</v>
       </c>
-      <c r="C15" s="1">
+      <c r="D16" s="1">
         <v>512915</v>
       </c>
-      <c r="D15" s="1">
+      <c r="E16" s="1">
         <v>512195</v>
       </c>
-      <c r="E15" s="1">
+      <c r="F16" s="1">
         <v>512196</v>
       </c>
-      <c r="F15" s="1">
+      <c r="G16" s="1">
         <v>512195</v>
       </c>
-      <c r="G15" s="1">
+      <c r="H16" s="1">
         <f t="shared" si="0"/>
         <v>512339.20000000001</v>
       </c>
-      <c r="H15" s="1">
-        <f t="shared" ref="H15:I15" si="25">G15/1000</f>
+      <c r="I16" s="1">
+        <f t="shared" ref="I16:J16" si="25">H16/1000</f>
         <v>512.33920000000001</v>
       </c>
-      <c r="I15" s="16">
+      <c r="J16" s="15">
         <f t="shared" si="25"/>
         <v>0.51233919999999999</v>
       </c>
-      <c r="J15" s="1">
-        <f t="shared" ref="J15:K15" si="26">I15/60</f>
+      <c r="K16" s="1">
+        <f t="shared" ref="K16:L16" si="26">J16/60</f>
         <v>8.5389866666666665E-3</v>
       </c>
-      <c r="K15" s="3">
+      <c r="L16" s="3">
         <f t="shared" si="26"/>
         <v>1.4231644444444443E-4</v>
       </c>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A16" s="2">
+    <row r="17" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="B17" s="2">
         <v>16</v>
       </c>
-      <c r="B16" s="1">
+      <c r="C17" s="1">
         <v>1255234</v>
       </c>
-      <c r="C16" s="1">
+      <c r="D17" s="1">
         <v>1255233</v>
       </c>
-      <c r="D16" s="1">
+      <c r="E17" s="1">
         <v>1255234</v>
       </c>
-      <c r="E16" s="1">
+      <c r="F17" s="1">
         <v>1255234</v>
       </c>
-      <c r="F16" s="1">
+      <c r="G17" s="1">
         <v>1255234</v>
       </c>
-      <c r="G16" s="1">
+      <c r="H17" s="1">
         <f t="shared" si="0"/>
         <v>1255233.8</v>
       </c>
-      <c r="H16" s="1">
-        <f t="shared" ref="H16:I16" si="27">G16/1000</f>
+      <c r="I17" s="1">
+        <f t="shared" ref="I17:J17" si="27">H17/1000</f>
         <v>1255.2338</v>
       </c>
-      <c r="I16" s="16">
+      <c r="J17" s="15">
         <f t="shared" si="27"/>
         <v>1.2552338000000001</v>
       </c>
-      <c r="J16" s="1">
-        <f t="shared" ref="J16:K16" si="28">I16/60</f>
+      <c r="K17" s="1">
+        <f t="shared" ref="K17:L17" si="28">J17/60</f>
         <v>2.0920563333333333E-2</v>
       </c>
-      <c r="K16" s="3">
+      <c r="L17" s="3">
         <f t="shared" si="28"/>
         <v>3.4867605555555557E-4</v>
       </c>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A17" s="2">
+    <row r="18" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="B18" s="2">
         <v>17</v>
       </c>
-      <c r="B17" s="1">
+      <c r="C18" s="1">
         <v>2741311</v>
       </c>
-      <c r="C17" s="1">
+      <c r="D18" s="1">
         <v>2741310</v>
       </c>
-      <c r="D17" s="1">
+      <c r="E18" s="1">
         <v>2741311</v>
       </c>
-      <c r="E17" s="1">
+      <c r="F18" s="1">
         <v>2741311</v>
       </c>
-      <c r="F17" s="1">
+      <c r="G18" s="1">
         <v>2741311</v>
       </c>
-      <c r="G17" s="1">
+      <c r="H18" s="1">
         <f t="shared" si="0"/>
         <v>2741310.8</v>
       </c>
-      <c r="H17" s="1">
-        <f t="shared" ref="H17:I17" si="29">G17/1000</f>
+      <c r="I18" s="1">
+        <f t="shared" ref="I18:J18" si="29">H18/1000</f>
         <v>2741.3107999999997</v>
       </c>
-      <c r="I17" s="16">
+      <c r="J18" s="15">
         <f t="shared" si="29"/>
         <v>2.7413107999999999</v>
       </c>
-      <c r="J17" s="1">
-        <f t="shared" ref="J17:K17" si="30">I17/60</f>
+      <c r="K18" s="1">
+        <f t="shared" ref="K18:L18" si="30">J18/60</f>
         <v>4.5688513333333333E-2</v>
       </c>
-      <c r="K17" s="3">
+      <c r="L18" s="3">
         <f t="shared" si="30"/>
         <v>7.6147522222222224E-4</v>
       </c>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A18" s="2">
+    <row r="19" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="B19" s="2">
         <v>18</v>
       </c>
-      <c r="B18" s="1">
+      <c r="C19" s="1">
         <v>5713464</v>
       </c>
-      <c r="C18" s="1">
+      <c r="D19" s="1">
         <v>5713465</v>
       </c>
-      <c r="D18" s="1">
+      <c r="E19" s="1">
         <v>5713465</v>
       </c>
-      <c r="E18" s="1">
+      <c r="F19" s="1">
         <v>5713466</v>
       </c>
-      <c r="F18" s="1">
+      <c r="G19" s="1">
         <v>5713465</v>
       </c>
-      <c r="G18" s="1">
+      <c r="H19" s="1">
         <f t="shared" si="0"/>
         <v>5713465</v>
       </c>
-      <c r="H18" s="1">
-        <f t="shared" ref="H18:I18" si="31">G18/1000</f>
+      <c r="I19" s="1">
+        <f t="shared" ref="I19:J19" si="31">H19/1000</f>
         <v>5713.4650000000001</v>
       </c>
-      <c r="I18" s="16">
+      <c r="J19" s="15">
         <f t="shared" si="31"/>
         <v>5.7134650000000002</v>
       </c>
-      <c r="J18" s="1">
-        <f t="shared" ref="J18:K18" si="32">I18/60</f>
+      <c r="K19" s="1">
+        <f t="shared" ref="K19:L19" si="32">J19/60</f>
         <v>9.5224416666666672E-2</v>
       </c>
-      <c r="K18" s="3">
+      <c r="L19" s="3">
         <f t="shared" si="32"/>
         <v>1.5870736111111112E-3</v>
       </c>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A19" s="2">
+    <row r="20" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="B20" s="2">
         <v>19</v>
       </c>
-      <c r="B19" s="1">
+      <c r="C20" s="1">
         <v>11657773</v>
       </c>
-      <c r="C19" s="1">
+      <c r="D20" s="1">
         <v>11657773</v>
       </c>
-      <c r="D19" s="1">
+      <c r="E20" s="1">
         <v>11657773</v>
       </c>
-      <c r="E19" s="1">
+      <c r="F20" s="1">
         <v>11657773</v>
       </c>
-      <c r="F19" s="1">
+      <c r="G20" s="1">
         <v>11657773</v>
       </c>
-      <c r="G19" s="1">
+      <c r="H20" s="1">
         <f t="shared" si="0"/>
         <v>11657773</v>
       </c>
-      <c r="H19" s="1">
-        <f t="shared" ref="H19:I19" si="33">G19/1000</f>
+      <c r="I20" s="1">
+        <f t="shared" ref="I20:J20" si="33">H20/1000</f>
         <v>11657.772999999999</v>
       </c>
-      <c r="I19" s="16">
+      <c r="J20" s="15">
         <f t="shared" si="33"/>
         <v>11.657772999999999</v>
       </c>
-      <c r="J19" s="1">
-        <f t="shared" ref="J19:K19" si="34">I19/60</f>
+      <c r="K20" s="1">
+        <f t="shared" ref="K20:L20" si="34">J20/60</f>
         <v>0.19429621666666666</v>
       </c>
-      <c r="K19" s="3">
+      <c r="L20" s="3">
         <f t="shared" si="34"/>
         <v>3.2382702777777775E-3</v>
       </c>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A20" s="2">
+    <row r="21" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="B21" s="2">
         <v>20</v>
       </c>
-      <c r="B20" s="1">
+      <c r="C21" s="1">
         <v>23546389</v>
       </c>
-      <c r="C20" s="1">
+      <c r="D21" s="1">
         <v>23546390</v>
       </c>
-      <c r="D20" s="1">
+      <c r="E21" s="1">
         <v>23546389</v>
       </c>
-      <c r="E20" s="1">
+      <c r="F21" s="1">
         <v>23546390</v>
       </c>
-      <c r="F20" s="1">
+      <c r="G21" s="1">
         <v>23546390</v>
       </c>
-      <c r="G20" s="1">
+      <c r="H21" s="1">
         <f t="shared" si="0"/>
         <v>23546389.600000001</v>
       </c>
-      <c r="H20" s="1">
-        <f t="shared" ref="H20:I20" si="35">G20/1000</f>
+      <c r="I21" s="1">
+        <f t="shared" ref="I21:J21" si="35">H21/1000</f>
         <v>23546.389600000002</v>
       </c>
-      <c r="I20" s="16">
+      <c r="J21" s="15">
         <f t="shared" si="35"/>
         <v>23.546389600000001</v>
       </c>
-      <c r="J20" s="1">
-        <f t="shared" ref="J20:K20" si="36">I20/60</f>
+      <c r="K21" s="1">
+        <f t="shared" ref="K21:L21" si="36">J21/60</f>
         <v>0.39243982666666671</v>
       </c>
-      <c r="K20" s="3">
+      <c r="L21" s="3">
         <f t="shared" si="36"/>
         <v>6.5406637777777783E-3</v>
       </c>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A21" s="2">
+    <row r="22" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="B22" s="2">
         <v>21</v>
       </c>
-      <c r="B21" s="1">
+      <c r="C22" s="1">
         <v>47323624</v>
       </c>
-      <c r="C21" s="1">
+      <c r="D22" s="1">
         <v>47323664</v>
       </c>
-      <c r="D21" s="1">
+      <c r="E22" s="1">
         <v>47323624</v>
       </c>
-      <c r="E21" s="1">
+      <c r="F22" s="1">
         <v>47323624</v>
       </c>
-      <c r="F21" s="1">
+      <c r="G22" s="1">
         <v>47323624</v>
       </c>
-      <c r="G21" s="1">
+      <c r="H22" s="1">
         <f t="shared" si="0"/>
         <v>47323632</v>
       </c>
-      <c r="H21" s="1">
-        <f t="shared" ref="H21:I21" si="37">G21/1000</f>
+      <c r="I22" s="1">
+        <f t="shared" ref="I22:J22" si="37">H22/1000</f>
         <v>47323.631999999998</v>
       </c>
-      <c r="I21" s="16">
+      <c r="J22" s="15">
         <f t="shared" si="37"/>
         <v>47.323631999999996</v>
       </c>
-      <c r="J21" s="1">
-        <f t="shared" ref="J21:K21" si="38">I21/60</f>
+      <c r="K22" s="1">
+        <f t="shared" ref="K22:L22" si="38">J22/60</f>
         <v>0.78872719999999996</v>
       </c>
-      <c r="K21" s="3">
+      <c r="L22" s="3">
         <f t="shared" si="38"/>
         <v>1.3145453333333333E-2</v>
       </c>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A22" s="2">
+    <row r="23" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="B23" s="2">
         <v>22</v>
       </c>
-      <c r="B22" s="1">
+      <c r="C23" s="1">
         <v>94878091</v>
       </c>
-      <c r="C22" s="1">
+      <c r="D23" s="1">
         <v>94878090</v>
       </c>
-      <c r="D22" s="1">
+      <c r="E23" s="1">
         <v>94878091</v>
       </c>
-      <c r="E22" s="1">
+      <c r="F23" s="1">
         <v>94878091</v>
       </c>
-      <c r="F22" s="1">
+      <c r="G23" s="1">
         <v>94878091</v>
       </c>
-      <c r="G22" s="1">
+      <c r="H23" s="1">
         <f t="shared" si="0"/>
         <v>94878090.799999997</v>
       </c>
-      <c r="H22" s="1">
-        <f t="shared" ref="H22:I22" si="39">G22/1000</f>
+      <c r="I23" s="1">
+        <f t="shared" ref="I23:J23" si="39">H23/1000</f>
         <v>94878.090799999991</v>
       </c>
-      <c r="I22" s="16">
+      <c r="J23" s="15">
         <f t="shared" si="39"/>
         <v>94.878090799999995</v>
       </c>
-      <c r="J22" s="1">
-        <f t="shared" ref="J22:K22" si="40">I22/60</f>
+      <c r="K23" s="1">
+        <f t="shared" ref="K23:L23" si="40">J23/60</f>
         <v>1.5813015133333332</v>
       </c>
-      <c r="K22" s="3">
+      <c r="L23" s="3">
         <f t="shared" si="40"/>
         <v>2.635502522222222E-2</v>
       </c>
     </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A23" s="2">
+    <row r="24" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="B24" s="2">
         <v>23</v>
       </c>
-      <c r="B23" s="1">
+      <c r="C24" s="1">
         <v>189987025</v>
       </c>
-      <c r="C23" s="1">
+      <c r="D24" s="1">
         <v>189987025</v>
       </c>
-      <c r="D23" s="1">
+      <c r="E24" s="1">
         <v>189987025</v>
       </c>
-      <c r="E23" s="1">
+      <c r="F24" s="1">
         <v>189987025</v>
       </c>
-      <c r="F23" s="1">
+      <c r="G24" s="1">
         <v>189987026</v>
       </c>
-      <c r="G23" s="1">
+      <c r="H24" s="1">
         <f t="shared" si="0"/>
         <v>189987025.19999999</v>
       </c>
-      <c r="H23" s="1">
-        <f t="shared" ref="H23:I23" si="41">G23/1000</f>
+      <c r="I24" s="1">
+        <f t="shared" ref="I24:J24" si="41">H24/1000</f>
         <v>189987.02519999997</v>
       </c>
-      <c r="I23" s="16">
+      <c r="J24" s="15">
         <f t="shared" si="41"/>
         <v>189.98702519999998</v>
       </c>
-      <c r="J23" s="1">
-        <f t="shared" ref="J23:K23" si="42">I23/60</f>
+      <c r="K24" s="1">
+        <f t="shared" ref="K24:L24" si="42">J24/60</f>
         <v>3.1664504199999994</v>
       </c>
-      <c r="K23" s="3">
+      <c r="L24" s="3">
         <f t="shared" si="42"/>
         <v>5.277417366666666E-2</v>
       </c>
     </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A24" s="2">
+    <row r="25" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="B25" s="2">
         <v>24</v>
       </c>
-      <c r="B24" s="1">
+      <c r="C25" s="1">
         <v>380204892</v>
       </c>
-      <c r="C24" s="1">
+      <c r="D25" s="1">
         <v>380204893</v>
       </c>
-      <c r="D24" s="1">
+      <c r="E25" s="1">
         <v>380204892</v>
       </c>
-      <c r="E24" s="1">
+      <c r="F25" s="1">
         <v>380204893</v>
       </c>
-      <c r="F24" s="1">
+      <c r="G25" s="1">
         <v>380204894</v>
       </c>
-      <c r="G24" s="1">
+      <c r="H25" s="1">
         <f t="shared" si="0"/>
         <v>380204892.80000001</v>
       </c>
-      <c r="H24" s="1">
-        <f t="shared" ref="H24:I24" si="43">G24/1000</f>
+      <c r="I25" s="1">
+        <f t="shared" ref="I25:J25" si="43">H25/1000</f>
         <v>380204.89280000003</v>
       </c>
-      <c r="I24" s="16">
+      <c r="J25" s="15">
         <f t="shared" si="43"/>
         <v>380.20489280000004</v>
       </c>
-      <c r="J24" s="1">
-        <f t="shared" ref="J24:K24" si="44">I24/60</f>
+      <c r="K25" s="1">
+        <f t="shared" ref="K25:L25" si="44">J25/60</f>
         <v>6.3367482133333342</v>
       </c>
-      <c r="K24" s="3">
+      <c r="L25" s="3">
         <f t="shared" si="44"/>
         <v>0.10561247022222224</v>
       </c>
     </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A25" s="2">
+    <row r="26" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="B26" s="2">
         <v>25</v>
       </c>
-      <c r="B25" s="1">
+      <c r="C26" s="1">
         <v>760636942</v>
       </c>
-      <c r="C25" s="1"/>
-      <c r="D25" s="1"/>
-      <c r="E25" s="1"/>
-      <c r="F25" s="1"/>
-      <c r="G25" s="1">
-        <f>SUM(B25:F25)</f>
-        <v>760636942</v>
-      </c>
-      <c r="H25" s="1">
-        <f t="shared" ref="H25:I25" si="45">G25/1000</f>
-        <v>760636.94200000004</v>
-      </c>
-      <c r="I25" s="16">
-        <f t="shared" si="45"/>
-        <v>760.63694200000009</v>
-      </c>
-      <c r="J25" s="1">
-        <f t="shared" ref="J25:K25" si="46">I25/60</f>
-        <v>12.677282366666669</v>
-      </c>
-      <c r="K25" s="3">
-        <f t="shared" si="46"/>
-        <v>0.21128803944444446</v>
-      </c>
-    </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A26" s="2">
-        <v>26</v>
-      </c>
-      <c r="B26" s="14">
-        <v>1521511257</v>
-      </c>
-      <c r="C26" s="1"/>
       <c r="D26" s="1"/>
       <c r="E26" s="1"/>
       <c r="F26" s="1"/>
-      <c r="G26" s="1">
-        <f t="shared" ref="G26:G32" si="47">SUM(B26:F26)</f>
+      <c r="G26" s="1"/>
+      <c r="H26" s="1">
+        <f>SUM(C26:G26)</f>
+        <v>760636942</v>
+      </c>
+      <c r="I26" s="1">
+        <f t="shared" ref="I26:J26" si="45">H26/1000</f>
+        <v>760636.94200000004</v>
+      </c>
+      <c r="J26" s="15">
+        <f t="shared" si="45"/>
+        <v>760.63694200000009</v>
+      </c>
+      <c r="K26" s="1">
+        <f t="shared" ref="K26:L26" si="46">J26/60</f>
+        <v>12.677282366666669</v>
+      </c>
+      <c r="L26" s="3">
+        <f t="shared" si="46"/>
+        <v>0.21128803944444446</v>
+      </c>
+    </row>
+    <row r="27" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="B27" s="2">
+        <v>26</v>
+      </c>
+      <c r="C27" s="18">
         <v>1521511257</v>
       </c>
-      <c r="H26" s="1">
-        <f t="shared" ref="H26:I26" si="48">G26/1000</f>
-        <v>1521511.257</v>
-      </c>
-      <c r="I26" s="16">
-        <f t="shared" si="48"/>
-        <v>1521.5112569999999</v>
-      </c>
-      <c r="J26" s="1">
-        <f t="shared" ref="J26:K26" si="49">I26/60</f>
-        <v>25.358520949999999</v>
-      </c>
-      <c r="K26" s="3">
-        <f t="shared" si="49"/>
-        <v>0.42264201583333333</v>
-      </c>
-    </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A27" s="2">
-        <v>27</v>
-      </c>
-      <c r="B27" s="1">
-        <v>3043253279</v>
-      </c>
-      <c r="C27" s="1"/>
       <c r="D27" s="1"/>
       <c r="E27" s="1"/>
       <c r="F27" s="1"/>
-      <c r="G27" s="1">
-        <f t="shared" si="47"/>
+      <c r="G27" s="1"/>
+      <c r="H27" s="1">
+        <f t="shared" ref="H27:H33" si="47">SUM(C27:G27)</f>
+        <v>1521511257</v>
+      </c>
+      <c r="I27" s="1">
+        <f t="shared" ref="I27:J27" si="48">H27/1000</f>
+        <v>1521511.257</v>
+      </c>
+      <c r="J27" s="15">
+        <f t="shared" si="48"/>
+        <v>1521.5112569999999</v>
+      </c>
+      <c r="K27" s="1">
+        <f t="shared" ref="K27:L27" si="49">J27/60</f>
+        <v>25.358520949999999</v>
+      </c>
+      <c r="L27" s="3">
+        <f t="shared" si="49"/>
+        <v>0.42264201583333333</v>
+      </c>
+    </row>
+    <row r="28" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="B28" s="2">
+        <v>27</v>
+      </c>
+      <c r="C28" s="1">
         <v>3043253279</v>
       </c>
-      <c r="H27" s="1">
-        <f t="shared" ref="H27:I27" si="50">G27/1000</f>
-        <v>3043253.2790000001</v>
-      </c>
-      <c r="I27" s="16">
-        <f t="shared" si="50"/>
-        <v>3043.253279</v>
-      </c>
-      <c r="J27" s="1">
-        <f t="shared" ref="J27:K27" si="51">I27/60</f>
-        <v>50.720887983333334</v>
-      </c>
-      <c r="K27" s="3">
-        <f t="shared" si="51"/>
-        <v>0.84534813305555556</v>
-      </c>
-    </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A28" s="2">
-        <v>28</v>
-      </c>
-      <c r="B28" s="1">
-        <f>B27*2+118356</f>
-        <v>6086624914</v>
-      </c>
-      <c r="C28" s="1"/>
       <c r="D28" s="1"/>
       <c r="E28" s="1"/>
       <c r="F28" s="1"/>
-      <c r="G28" s="1">
+      <c r="G28" s="1"/>
+      <c r="H28" s="1">
         <f t="shared" si="47"/>
+        <v>3043253279</v>
+      </c>
+      <c r="I28" s="1">
+        <f t="shared" ref="I28:J28" si="50">H28/1000</f>
+        <v>3043253.2790000001</v>
+      </c>
+      <c r="J28" s="15">
+        <f t="shared" si="50"/>
+        <v>3043.253279</v>
+      </c>
+      <c r="K28" s="1">
+        <f t="shared" ref="K28:L28" si="51">J28/60</f>
+        <v>50.720887983333334</v>
+      </c>
+      <c r="L28" s="3">
+        <f t="shared" si="51"/>
+        <v>0.84534813305555556</v>
+      </c>
+    </row>
+    <row r="29" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="B29" s="2">
+        <v>28</v>
+      </c>
+      <c r="C29" s="1">
+        <f>C28*2+118356</f>
         <v>6086624914</v>
       </c>
-      <c r="H28" s="1">
-        <f t="shared" ref="H28:I28" si="52">G28/1000</f>
-        <v>6086624.9139999999</v>
-      </c>
-      <c r="I28" s="16">
-        <f t="shared" si="52"/>
-        <v>6086.624914</v>
-      </c>
-      <c r="J28" s="1">
-        <f t="shared" ref="J28:K28" si="53">I28/60</f>
-        <v>101.44374856666667</v>
-      </c>
-      <c r="K28" s="3">
-        <f t="shared" si="53"/>
-        <v>1.6907291427777777</v>
-      </c>
-    </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A29" s="2">
-        <v>29</v>
-      </c>
-      <c r="B29" s="1">
-        <f t="shared" ref="B29:B32" si="54">B28*2+118356</f>
-        <v>12173368184</v>
-      </c>
-      <c r="C29" s="1"/>
       <c r="D29" s="1"/>
       <c r="E29" s="1"/>
       <c r="F29" s="1"/>
-      <c r="G29" s="1">
+      <c r="G29" s="1"/>
+      <c r="H29" s="1">
         <f t="shared" si="47"/>
+        <v>6086624914</v>
+      </c>
+      <c r="I29" s="1">
+        <f t="shared" ref="I29:J29" si="52">H29/1000</f>
+        <v>6086624.9139999999</v>
+      </c>
+      <c r="J29" s="15">
+        <f t="shared" si="52"/>
+        <v>6086.624914</v>
+      </c>
+      <c r="K29" s="1">
+        <f t="shared" ref="K29:L29" si="53">J29/60</f>
+        <v>101.44374856666667</v>
+      </c>
+      <c r="L29" s="3">
+        <f t="shared" si="53"/>
+        <v>1.6907291427777777</v>
+      </c>
+    </row>
+    <row r="30" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="B30" s="2">
+        <v>29</v>
+      </c>
+      <c r="C30" s="17">
+        <f t="shared" ref="C30:C33" si="54">C29*2+118356</f>
         <v>12173368184</v>
       </c>
-      <c r="H29" s="1">
-        <f t="shared" ref="H29:I29" si="55">G29/1000</f>
-        <v>12173368.184</v>
-      </c>
-      <c r="I29" s="16">
-        <f t="shared" si="55"/>
-        <v>12173.368184000001</v>
-      </c>
-      <c r="J29" s="1">
-        <f t="shared" ref="J29:K29" si="56">I29/60</f>
-        <v>202.88946973333336</v>
-      </c>
-      <c r="K29" s="3">
-        <f t="shared" si="56"/>
-        <v>3.3814911622222228</v>
-      </c>
-    </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A30" s="2">
-        <v>30</v>
-      </c>
-      <c r="B30" s="1">
-        <f t="shared" si="54"/>
-        <v>24346854724</v>
-      </c>
-      <c r="C30" s="1"/>
       <c r="D30" s="1"/>
       <c r="E30" s="1"/>
       <c r="F30" s="1"/>
-      <c r="G30" s="1">
+      <c r="G30" s="1"/>
+      <c r="H30" s="1">
         <f t="shared" si="47"/>
+        <v>12173368184</v>
+      </c>
+      <c r="I30" s="1">
+        <f t="shared" ref="I30:J30" si="55">H30/1000</f>
+        <v>12173368.184</v>
+      </c>
+      <c r="J30" s="15">
+        <f t="shared" si="55"/>
+        <v>12173.368184000001</v>
+      </c>
+      <c r="K30" s="1">
+        <f t="shared" ref="K30:L30" si="56">J30/60</f>
+        <v>202.88946973333336</v>
+      </c>
+      <c r="L30" s="3">
+        <f t="shared" si="56"/>
+        <v>3.3814911622222228</v>
+      </c>
+    </row>
+    <row r="31" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="B31" s="2">
+        <v>30</v>
+      </c>
+      <c r="C31" s="17">
+        <f t="shared" si="54"/>
         <v>24346854724</v>
       </c>
-      <c r="H30" s="1">
-        <f t="shared" ref="H30:I30" si="57">G30/1000</f>
-        <v>24346854.723999999</v>
-      </c>
-      <c r="I30" s="16">
-        <f t="shared" si="57"/>
-        <v>24346.854724000001</v>
-      </c>
-      <c r="J30" s="1">
-        <f t="shared" ref="J30:K30" si="58">I30/60</f>
-        <v>405.7809120666667</v>
-      </c>
-      <c r="K30" s="3">
-        <f t="shared" si="58"/>
-        <v>6.763015201111112</v>
-      </c>
-    </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A31" s="2">
-        <v>31</v>
-      </c>
-      <c r="B31" s="1">
-        <f t="shared" si="54"/>
-        <v>48693827804</v>
-      </c>
-      <c r="C31" s="1"/>
       <c r="D31" s="1"/>
       <c r="E31" s="1"/>
       <c r="F31" s="1"/>
-      <c r="G31" s="1">
+      <c r="G31" s="1"/>
+      <c r="H31" s="1">
+        <f t="shared" si="47"/>
+        <v>24346854724</v>
+      </c>
+      <c r="I31" s="1">
+        <f t="shared" ref="I31:J31" si="57">H31/1000</f>
+        <v>24346854.723999999</v>
+      </c>
+      <c r="J31" s="15">
+        <f t="shared" si="57"/>
+        <v>24346.854724000001</v>
+      </c>
+      <c r="K31" s="1">
+        <f t="shared" ref="K31:L31" si="58">J31/60</f>
+        <v>405.7809120666667</v>
+      </c>
+      <c r="L31" s="3">
+        <f t="shared" si="58"/>
+        <v>6.763015201111112</v>
+      </c>
+    </row>
+    <row r="32" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="B32" s="2">
+        <v>31</v>
+      </c>
+      <c r="C32" s="17">
+        <f t="shared" si="54"/>
+        <v>48693827804</v>
+      </c>
+      <c r="D32" s="1"/>
+      <c r="E32" s="1"/>
+      <c r="F32" s="1"/>
+      <c r="G32" s="1"/>
+      <c r="H32" s="1">
         <f t="shared" si="47"/>
         <v>48693827804</v>
       </c>
-      <c r="H31" s="1">
-        <f t="shared" ref="H31:I31" si="59">G31/1000</f>
+      <c r="I32" s="1">
+        <f t="shared" ref="I32:J32" si="59">H32/1000</f>
         <v>48693827.803999998</v>
       </c>
-      <c r="I31" s="16">
+      <c r="J32" s="15">
         <f t="shared" si="59"/>
         <v>48693.827804</v>
       </c>
-      <c r="J31" s="1">
-        <f t="shared" ref="J31:K31" si="60">I31/60</f>
+      <c r="K32" s="1">
+        <f t="shared" ref="K32:L32" si="60">J32/60</f>
         <v>811.56379673333333</v>
       </c>
-      <c r="K31" s="3">
+      <c r="L32" s="3">
         <f t="shared" si="60"/>
         <v>13.526063278888889</v>
       </c>
     </row>
-    <row r="32" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A32" s="4">
+    <row r="33" spans="2:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B33" s="4">
         <v>32</v>
       </c>
-      <c r="B32" s="1">
+      <c r="C33" s="19">
         <f t="shared" si="54"/>
         <v>97387773964</v>
       </c>
-      <c r="C32" s="5"/>
-      <c r="D32" s="5"/>
-      <c r="E32" s="5"/>
-      <c r="F32" s="5"/>
-      <c r="G32" s="5">
+      <c r="D33" s="5"/>
+      <c r="E33" s="5"/>
+      <c r="F33" s="5"/>
+      <c r="G33" s="5"/>
+      <c r="H33" s="5">
         <f t="shared" si="47"/>
         <v>97387773964</v>
       </c>
-      <c r="H32" s="5">
-        <f t="shared" ref="H32:I32" si="61">G32/1000</f>
+      <c r="I33" s="5">
+        <f t="shared" ref="I33:J33" si="61">H33/1000</f>
         <v>97387773.964000002</v>
       </c>
-      <c r="I32" s="17">
+      <c r="J33" s="16">
         <f t="shared" si="61"/>
         <v>97387.773964000007</v>
       </c>
-      <c r="J32" s="5">
-        <f t="shared" ref="J32:K32" si="62">I32/60</f>
+      <c r="K33" s="5">
+        <f t="shared" ref="K33:L33" si="62">J33/60</f>
         <v>1623.1295660666667</v>
       </c>
-      <c r="K32" s="6">
+      <c r="L33" s="6">
         <f t="shared" si="62"/>
         <v>27.052159434444444</v>
       </c>

</xml_diff>